<commit_message>
Allow for inputs other than phase and period
</commit_message>
<xml_diff>
--- a/server_code/test.xlsx
+++ b/server_code/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adalessa/Projects/2050Calc/anvil/Test_Dashboard/server_code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adalessa/Projects/2050Calc/anvil/Template2050Calculator/server_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5B35BC-D43D-7B40-8FF3-F87858CF5BBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3EFD85-DBD6-0140-AD77-F94028BBAB68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{E3E7D5AE-718D-4492-A5CF-364461443CE4}"/>
   </bookViews>
@@ -16,13 +16,15 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="INPUT.amplitude">Sheet1!$A$3</definedName>
     <definedName name="INPUT.PERIOD">Sheet1!$A$1</definedName>
     <definedName name="INPUT.PHASE">Sheet1!$A$2</definedName>
-    <definedName name="output.cos">Sheet1!$A$6:$U$6</definedName>
-    <definedName name="output.sin">Sheet1!$A$5:$U$5</definedName>
-    <definedName name="output.x">Sheet1!$A$4:$U$4</definedName>
+    <definedName name="output.arctan">Sheet1!$A$8:$U$8</definedName>
+    <definedName name="output.cos">Sheet1!$A$7:$U$7</definedName>
+    <definedName name="output.sin">Sheet1!$A$6:$U$6</definedName>
+    <definedName name="output.x">Sheet1!$A$5:$U$5</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -386,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE10450A-E94A-4F5E-8BAC-3DBE686CA3F0}">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:U4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -406,325 +408,416 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0.1</v>
-      </c>
-      <c r="C3">
-        <v>0.2</v>
-      </c>
-      <c r="D3">
-        <v>0.3</v>
-      </c>
-      <c r="E3">
-        <v>0.4</v>
-      </c>
-      <c r="F3">
-        <v>0.5</v>
-      </c>
-      <c r="G3">
-        <v>0.6</v>
-      </c>
-      <c r="H3">
-        <v>0.7</v>
-      </c>
-      <c r="I3">
-        <v>0.8</v>
-      </c>
-      <c r="J3">
-        <v>0.9</v>
-      </c>
-      <c r="K3">
         <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M3">
-        <v>1.2</v>
-      </c>
-      <c r="N3">
-        <v>1.3</v>
-      </c>
-      <c r="O3">
-        <v>1.4</v>
-      </c>
-      <c r="P3">
-        <v>1.5</v>
-      </c>
-      <c r="Q3">
-        <v>1.6</v>
-      </c>
-      <c r="R3">
-        <v>1.7</v>
-      </c>
-      <c r="S3">
-        <v>1.8</v>
-      </c>
-      <c r="T3">
-        <v>1.9</v>
-      </c>
-      <c r="U3">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f>A3*PI()</f>
         <v>0</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:U4" si="0">B3*PI()</f>
-        <v>0.31415926535897931</v>
+        <v>0.1</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>0.62831853071795862</v>
+        <v>0.2</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0.94247779607693793</v>
+        <v>0.3</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
-        <v>1.2566370614359172</v>
+        <v>0.4</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
-        <v>1.5707963267948966</v>
+        <v>0.5</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
-        <v>1.8849555921538759</v>
+        <v>0.6</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
-        <v>2.1991148575128552</v>
+        <v>0.7</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>2.5132741228718345</v>
+        <v>0.8</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
-        <v>2.8274333882308138</v>
+        <v>0.9</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
-        <v>3.1415926535897931</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
-        <v>3.4557519189487729</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
-        <v>3.7699111843077517</v>
+        <v>1.2</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
-        <v>4.0840704496667311</v>
+        <v>1.3</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
-        <v>4.3982297150257104</v>
+        <v>1.4</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
-        <v>4.7123889803846897</v>
+        <v>1.5</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="0"/>
-        <v>5.026548245743669</v>
+        <v>1.6</v>
       </c>
       <c r="R4">
-        <f t="shared" si="0"/>
-        <v>5.3407075111026483</v>
+        <v>1.7</v>
       </c>
       <c r="S4">
-        <f t="shared" si="0"/>
-        <v>5.6548667764616276</v>
+        <v>1.8</v>
       </c>
       <c r="T4">
-        <f t="shared" si="0"/>
-        <v>5.9690260418206069</v>
+        <v>1.9</v>
       </c>
       <c r="U4">
-        <f t="shared" si="0"/>
-        <v>6.2831853071795862</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f>SIN($A$1*A$4+$A$2)</f>
+        <f>A4*PI()</f>
         <v>0</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:U5" si="1">SIN($A$1*B$4+$A$2)</f>
-        <v>0.3090169943749474</v>
+        <f t="shared" ref="B5:U5" si="0">B4*PI()</f>
+        <v>0.31415926535897931</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
-        <v>0.58778525229247314</v>
+        <f t="shared" si="0"/>
+        <v>0.62831853071795862</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
-        <v>0.80901699437494745</v>
+        <f t="shared" si="0"/>
+        <v>0.94247779607693793</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
-        <v>0.95105651629515353</v>
+        <f t="shared" si="0"/>
+        <v>1.2566370614359172</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>1.5707963267948966</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
-        <v>0.95105651629515364</v>
+        <f t="shared" si="0"/>
+        <v>1.8849555921538759</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
-        <v>0.80901699437494745</v>
+        <f t="shared" si="0"/>
+        <v>2.1991148575128552</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
-        <v>0.58778525229247325</v>
+        <f t="shared" si="0"/>
+        <v>2.5132741228718345</v>
       </c>
       <c r="J5">
-        <f t="shared" si="1"/>
-        <v>0.30901699437494751</v>
+        <f t="shared" si="0"/>
+        <v>2.8274333882308138</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
-        <v>1.22514845490862E-16</v>
+        <f t="shared" si="0"/>
+        <v>3.1415926535897931</v>
       </c>
       <c r="L5">
-        <f t="shared" si="1"/>
-        <v>-0.30901699437494773</v>
+        <f t="shared" si="0"/>
+        <v>3.4557519189487729</v>
       </c>
       <c r="M5">
-        <f t="shared" si="1"/>
-        <v>-0.58778525229247303</v>
+        <f t="shared" si="0"/>
+        <v>3.7699111843077517</v>
       </c>
       <c r="N5">
-        <f t="shared" si="1"/>
-        <v>-0.80901699437494734</v>
+        <f t="shared" si="0"/>
+        <v>4.0840704496667311</v>
       </c>
       <c r="O5">
-        <f t="shared" si="1"/>
-        <v>-0.95105651629515353</v>
+        <f t="shared" si="0"/>
+        <v>4.3982297150257104</v>
       </c>
       <c r="P5">
-        <f t="shared" si="1"/>
-        <v>-1</v>
+        <f t="shared" si="0"/>
+        <v>4.7123889803846897</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="1"/>
-        <v>-0.95105651629515364</v>
+        <f t="shared" si="0"/>
+        <v>5.026548245743669</v>
       </c>
       <c r="R5">
-        <f t="shared" si="1"/>
-        <v>-0.80901699437494756</v>
+        <f t="shared" si="0"/>
+        <v>5.3407075111026483</v>
       </c>
       <c r="S5">
-        <f t="shared" si="1"/>
-        <v>-0.58778525229247336</v>
+        <f t="shared" si="0"/>
+        <v>5.6548667764616276</v>
       </c>
       <c r="T5">
-        <f t="shared" si="1"/>
-        <v>-0.30901699437494762</v>
+        <f t="shared" si="0"/>
+        <v>5.9690260418206069</v>
       </c>
       <c r="U5">
-        <f t="shared" si="1"/>
-        <v>-2.45029690981724E-16</v>
+        <f t="shared" si="0"/>
+        <v>6.2831853071795862</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6">
-        <f>COS($A$1*A$4+$A$2)</f>
+        <f>INPUT.amplitude*SIN($A$1*A$5+$A$2)</f>
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <f>INPUT.amplitude*SIN($A$1*B$5+$A$2)</f>
+        <v>0.3090169943749474</v>
+      </c>
+      <c r="C6">
+        <f>INPUT.amplitude*SIN($A$1*C$5+$A$2)</f>
+        <v>0.58778525229247314</v>
+      </c>
+      <c r="D6">
+        <f>INPUT.amplitude*SIN($A$1*D$5+$A$2)</f>
+        <v>0.80901699437494745</v>
+      </c>
+      <c r="E6">
+        <f>INPUT.amplitude*SIN($A$1*E$5+$A$2)</f>
+        <v>0.95105651629515353</v>
+      </c>
+      <c r="F6">
+        <f>INPUT.amplitude*SIN($A$1*F$5+$A$2)</f>
         <v>1</v>
       </c>
-      <c r="B6">
-        <f t="shared" ref="B6:U6" si="2">COS($A$1*B$4+$A$2)</f>
+      <c r="G6">
+        <f>INPUT.amplitude*SIN($A$1*G$5+$A$2)</f>
+        <v>0.95105651629515364</v>
+      </c>
+      <c r="H6">
+        <f>INPUT.amplitude*SIN($A$1*H$5+$A$2)</f>
+        <v>0.80901699437494745</v>
+      </c>
+      <c r="I6">
+        <f>INPUT.amplitude*SIN($A$1*I$5+$A$2)</f>
+        <v>0.58778525229247325</v>
+      </c>
+      <c r="J6">
+        <f>INPUT.amplitude*SIN($A$1*J$5+$A$2)</f>
+        <v>0.30901699437494751</v>
+      </c>
+      <c r="K6">
+        <f>INPUT.amplitude*SIN($A$1*K$5+$A$2)</f>
+        <v>1.22514845490862E-16</v>
+      </c>
+      <c r="L6">
+        <f>INPUT.amplitude*SIN($A$1*L$5+$A$2)</f>
+        <v>-0.30901699437494773</v>
+      </c>
+      <c r="M6">
+        <f>INPUT.amplitude*SIN($A$1*M$5+$A$2)</f>
+        <v>-0.58778525229247303</v>
+      </c>
+      <c r="N6">
+        <f>INPUT.amplitude*SIN($A$1*N$5+$A$2)</f>
+        <v>-0.80901699437494734</v>
+      </c>
+      <c r="O6">
+        <f>INPUT.amplitude*SIN($A$1*O$5+$A$2)</f>
+        <v>-0.95105651629515353</v>
+      </c>
+      <c r="P6">
+        <f>INPUT.amplitude*SIN($A$1*P$5+$A$2)</f>
+        <v>-1</v>
+      </c>
+      <c r="Q6">
+        <f>INPUT.amplitude*SIN($A$1*Q$5+$A$2)</f>
+        <v>-0.95105651629515364</v>
+      </c>
+      <c r="R6">
+        <f>INPUT.amplitude*SIN($A$1*R$5+$A$2)</f>
+        <v>-0.80901699437494756</v>
+      </c>
+      <c r="S6">
+        <f>INPUT.amplitude*SIN($A$1*S$5+$A$2)</f>
+        <v>-0.58778525229247336</v>
+      </c>
+      <c r="T6">
+        <f>INPUT.amplitude*SIN($A$1*T$5+$A$2)</f>
+        <v>-0.30901699437494762</v>
+      </c>
+      <c r="U6">
+        <f>INPUT.amplitude*SIN($A$1*U$5+$A$2)</f>
+        <v>-2.45029690981724E-16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f>$A$3*COS($A$1*A$5+$A$2)</f>
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ref="B7:U7" si="1">$A$3*COS($A$1*B$5+$A$2)</f>
         <v>0.95105651629515353</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="2"/>
+      <c r="C7">
+        <f t="shared" si="1"/>
         <v>0.80901699437494745</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="2"/>
+      <c r="D7">
+        <f t="shared" si="1"/>
         <v>0.58778525229247314</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="2"/>
+      <c r="E7">
+        <f t="shared" si="1"/>
         <v>0.30901699437494745</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="2"/>
+      <c r="F7">
+        <f t="shared" si="1"/>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="2"/>
+      <c r="G7">
+        <f t="shared" si="1"/>
         <v>-0.30901699437494734</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="2"/>
+      <c r="H7">
+        <f t="shared" si="1"/>
         <v>-0.58778525229247303</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="2"/>
+      <c r="I7">
+        <f t="shared" si="1"/>
         <v>-0.80901699437494734</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="2"/>
+      <c r="J7">
+        <f t="shared" si="1"/>
         <v>-0.95105651629515353</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="2"/>
+      <c r="K7">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="L6">
-        <f t="shared" si="2"/>
+      <c r="L7">
+        <f t="shared" si="1"/>
         <v>-0.95105651629515353</v>
       </c>
-      <c r="M6">
-        <f t="shared" si="2"/>
+      <c r="M7">
+        <f t="shared" si="1"/>
         <v>-0.80901699437494756</v>
       </c>
-      <c r="N6">
-        <f t="shared" si="2"/>
+      <c r="N7">
+        <f t="shared" si="1"/>
         <v>-0.58778525229247325</v>
       </c>
-      <c r="O6">
-        <f t="shared" si="2"/>
+      <c r="O7">
+        <f t="shared" si="1"/>
         <v>-0.30901699437494756</v>
       </c>
-      <c r="P6">
-        <f t="shared" si="2"/>
+      <c r="P7">
+        <f t="shared" si="1"/>
         <v>-1.83772268236293E-16</v>
       </c>
-      <c r="Q6">
-        <f t="shared" si="2"/>
+      <c r="Q7">
+        <f t="shared" si="1"/>
         <v>0.30901699437494723</v>
       </c>
-      <c r="R6">
-        <f t="shared" si="2"/>
+      <c r="R7">
+        <f t="shared" si="1"/>
         <v>0.58778525229247292</v>
       </c>
-      <c r="S6">
-        <f t="shared" si="2"/>
+      <c r="S7">
+        <f t="shared" si="1"/>
         <v>0.80901699437494734</v>
       </c>
-      <c r="T6">
-        <f t="shared" si="2"/>
+      <c r="T7">
+        <f t="shared" si="1"/>
         <v>0.95105651629515353</v>
       </c>
-      <c r="U6">
-        <f t="shared" si="2"/>
+      <c r="U7">
+        <f t="shared" si="1"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f>$A$3*ATAN($A$1*A$5+$A$2)</f>
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ref="B8:U8" si="2">$A$3*ATAN($A$1*B$5+$A$2)</f>
+        <v>0.30439579736461508</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>0.56098211610862381</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>0.75579401615930752</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>0.89863709305634221</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>1.0038848218538872</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>1.0830346193361855</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>1.1440172176193328</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>1.1921125187390871</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>1.2308489676792804</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>1.2626272556789118</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>1.2891177088292471</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>1.3115093180978645</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>1.3306670190047116</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="2"/>
+        <v>1.347232743213294</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>1.3616916829711636</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="2"/>
+        <v>1.3744166663632307</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="2"/>
+        <v>1.3856984864957245</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="2"/>
+        <v>1.3957670341481219</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="2"/>
+        <v>1.4048062895875966</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="2"/>
+        <v>1.4129651365067377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>